<commit_message>
Move the progress display before the inner rendering loop
</commit_message>
<xml_diff>
--- a/benchmark.xlsx
+++ b/benchmark.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dzutr\GitHub\Ray-Tracing-In-One-Weekend\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dzutrinh/Developer/Ray-Tracing-In-One-Weekend/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51A5E057-4F79-4C63-829F-3AA16A6C4163}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27F560E7-6600-3543-836C-70FEA78169B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{15C0AE52-249E-45FA-9761-9F30FDA75ADA}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14500" xr2:uid="{15C0AE52-249E-45FA-9761-9F30FDA75ADA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,17 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>System</t>
   </si>
@@ -39,9 +34,6 @@
   </si>
   <si>
     <t>OS</t>
-  </si>
-  <si>
-    <t>macOS High Sierra</t>
   </si>
   <si>
     <t xml:space="preserve">Windows 10 Pro Workstation </t>
@@ -75,6 +67,9 @@
   </si>
   <si>
     <t>Lower = Better</t>
+  </si>
+  <si>
+    <t>macOS Catalina</t>
   </si>
 </sst>
 </file>
@@ -198,7 +193,7 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Candara" panose="020E0502030303020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
@@ -230,7 +225,7 @@
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Candara" panose="020E0502030303020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
@@ -371,7 +366,7 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Candara" panose="020E0502030303020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
@@ -421,7 +416,7 @@
                         <a:lumOff val="35000"/>
                       </a:schemeClr>
                     </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
+                    <a:latin typeface="Candara" panose="020E0502030303020204" pitchFamily="34" charset="0"/>
                     <a:ea typeface="+mn-ea"/>
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
@@ -453,7 +448,7 @@
                       <a:lumOff val="35000"/>
                     </a:schemeClr>
                   </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
+                  <a:latin typeface="Candara" panose="020E0502030303020204" pitchFamily="34" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
@@ -485,7 +480,7 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Candara" panose="020E0502030303020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
@@ -536,7 +531,9 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr>
+          <a:latin typeface="Candara" panose="020E0502030303020204" pitchFamily="34" charset="0"/>
+        </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -1064,15 +1061,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>8929</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>595</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>330398</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>424656</xdr:colOff>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>76795</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1400,28 +1397,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B05104DC-DD03-4B6C-9F3F-6F1902AF08E7}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
@@ -1432,56 +1431,56 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="C5" s="2">
         <v>738.74</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C6" s="2">
         <v>804.04300000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C7" s="2">
         <v>1160.75</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C8" s="2">
         <v>1237.54</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C9" s="2">
         <v>1628.93</v>

</xml_diff>

<commit_message>
Benchmark updated. Permission fixed on Linux
</commit_message>
<xml_diff>
--- a/benchmark.xlsx
+++ b/benchmark.xlsx
@@ -70,7 +70,7 @@
     <t xml:space="preserve">Core i5-560M @ 2.6Ghz</t>
   </si>
   <si>
-    <t xml:space="preserve">Ubuntu 20.10</t>
+    <t xml:space="preserve">Ubuntu 22.04</t>
   </si>
 </sst>
 </file>
@@ -213,13 +213,14 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8359375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.84765625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="36.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.68"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -309,10 +310,24 @@
         <v>16</v>
       </c>
       <c r="C10" s="3" t="n">
-        <v>923.821</v>
+        <v>1005.79</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="C5:C10">
+    <cfRule type="dataBar" priority="2">
+      <dataBar showValue="1" minLength="0" maxLength="100">
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF2A6099"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{67ABB0F0-BBBD-4A51-B35B-7AF910CA342B}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -320,5 +335,22 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{67ABB0F0-BBBD-4A51-B35B-7AF910CA342B}">
+            <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="false">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>C5:C10</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>